<commit_message>
Fixed solenoid MOSFET hookup
</commit_message>
<xml_diff>
--- a/board/BOM with links.xlsx
+++ b/board/BOM with links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\GitHub\deploymentboard\board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DAD3AE1-59A7-4C46-80C3-78E7F11680B8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9DEE683E-46E5-4A4A-B8D0-1E4CEBAC6FA8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{C6344055-91BD-44FF-A542-68420F33CBC0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="139">
   <si>
     <t>Id</t>
   </si>
@@ -96,9 +96,6 @@
     <t>D_Small</t>
   </si>
   <si>
-    <t>R17,R14,R7,R13,R6,R4,R2,R1,R5</t>
-  </si>
-  <si>
     <t>R_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>C12</t>
   </si>
   <si>
-    <t>C_Small</t>
-  </si>
-  <si>
     <t>C11,C6</t>
   </si>
   <si>
@@ -249,15 +243,9 @@
     <t>27nH</t>
   </si>
   <si>
-    <t>D2,D1</t>
-  </si>
-  <si>
     <t>LED_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -279,12 +267,6 @@
     <t>432k</t>
   </si>
   <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
     <t>R9,R8</t>
   </si>
   <si>
@@ -394,6 +376,84 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/yageo/CC0603JRNPO9BN150/311-1060-1-ND/302970</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10B105MO8NNWC/1276-6524-1-ND/5961383</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10A226MO7JZNC/1276-7076-1-ND/7320718</t>
+  </si>
+  <si>
+    <t>R17,R14,R7,R13,R6,R4,R2,R1,R5,R10</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/susumu/RR0816P-103-D/RR08P10.0KDCT-ND/432748</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF22R0V/P22.0HCT-ND/1746745</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERA-3AEB4992V/P49.9KDBCT-ND/3075986</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC0603FR-07432KL/311-432KHRCT-ND/730186</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ270/RHM27DCT-ND/4053754</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC0603JR-0747KL/311-47KGRCT-ND/729741</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/taiyo-yuden/LBC3225T100KR/587-2421-1-ND/2230287</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/1277AS-H-4R7M=P2/490-10594-2-ND/5247205</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/tdk-corporation/NLV32T-027J-EF/445-16534-1-ND/4766575</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/jst-sales-america-inc/B2B-PH-K-S-LF-SN/455-1704-ND/926611</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/GRPB032MWCN-RC/S9017E-03-ND/1786480</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/pui-audio-inc/AT-1224-TWT-5V-2-R/668-1470-ND/5011404</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/jst-sales-america-inc/B3B-PH-K-S-LF-SN/455-1705-ND/926612</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Shappy-Pieces-Connector-Silicone-Female/dp/B07449V33P</t>
+  </si>
+  <si>
+    <t>JST connectors on cable (01x03)</t>
+  </si>
+  <si>
+    <t>JST Connectors on cable (01x02)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Micro-Connector-150mm-Cable-Female/dp/B01DUC1PW6</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/rohm-semiconductor/SML-D12M8WT86/511-1578-1-ND/1641810</t>
+  </si>
+  <si>
+    <t>LED - green</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/rohm-semiconductor/SML-310VTT86/511-1301-1-ND/637114</t>
+  </si>
+  <si>
+    <t>LED - red</t>
   </si>
 </sst>
 </file>
@@ -805,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A6BD62-FDD6-47EF-B9D6-52E19115CCE2}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,11 +918,12 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -878,11 +939,12 @@
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
+        <f t="shared" ref="A4:A27" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -897,12 +959,13 @@
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
+      <c r="F4" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -918,55 +981,58 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D6">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -975,38 +1041,40 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -1015,98 +1083,103 @@
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>9</v>
+      <c r="F13" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>9</v>
+      <c r="F14" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>11</v>
@@ -1115,18 +1188,19 @@
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>11</v>
@@ -1135,18 +1209,19 @@
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>11</v>
@@ -1155,18 +1230,19 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>11</v>
@@ -1177,16 +1253,17 @@
       <c r="E18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>9</v>
+      <c r="F18" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>11</v>
@@ -1195,18 +1272,19 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>11</v>
@@ -1215,366 +1293,399 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>9</v>
+        <v>52</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>21</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>23</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>9</v>
+      <c r="F24" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>25</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>9</v>
+        <v>65</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>27</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>123</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>9</v>
+        <v>136</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>28</v>
+        <f>A27+1</f>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>75</v>
+        <v>138</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>29</v>
+        <f>A28+1</f>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>9</v>
+        <v>71</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>30</v>
+        <f t="shared" ref="A30:A37" si="1">A29+1</f>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>9</v>
+        <v>73</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>9</v>
+        <v>77</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>9</v>
+        <v>79</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>35</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D35">
         <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E40" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>133</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>132</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1586,7 +1697,7 @@
     <hyperlink ref="F36" r:id="rId5" xr:uid="{14114C7B-35A6-4B40-BB43-C704ABA7C9A6}"/>
     <hyperlink ref="F12" r:id="rId6" xr:uid="{2EE0D797-549B-4A6D-9223-33FA19CB546F}"/>
     <hyperlink ref="F39" r:id="rId7" xr:uid="{CE9755CD-C731-43CE-845F-FE1172B8F4C6}"/>
-    <hyperlink ref="F28" r:id="rId8" xr:uid="{7A9698D1-D72F-4EE7-A37B-A936EBAA0814}"/>
+    <hyperlink ref="F29" r:id="rId8" xr:uid="{7A9698D1-D72F-4EE7-A37B-A936EBAA0814}"/>
     <hyperlink ref="F22" r:id="rId9" xr:uid="{527BDBE7-EDB4-4F1C-8C3A-D5F6CDC8604E}"/>
     <hyperlink ref="F23" r:id="rId10" xr:uid="{796E59D9-C24A-4BB4-87BF-4227F49F297B}"/>
     <hyperlink ref="F40" r:id="rId11" xr:uid="{E07C1A4E-13BC-4BFA-BB10-AA2660FC8215}"/>
@@ -1598,10 +1709,31 @@
     <hyperlink ref="F15" r:id="rId17" xr:uid="{8ED21990-D041-4B2D-B1EF-6B402B2D6474}"/>
     <hyperlink ref="F16" r:id="rId18" xr:uid="{3A1908C1-BD15-4C0D-8F20-1DBCF6156438}"/>
     <hyperlink ref="F17" r:id="rId19" xr:uid="{C0BE36CC-CFE9-4E1E-A546-291FCA536A30}"/>
+    <hyperlink ref="F18" r:id="rId20" xr:uid="{38C4619F-664A-4180-B357-A0291DC73733}"/>
+    <hyperlink ref="F19" r:id="rId21" xr:uid="{249D289D-D515-46ED-A6C1-7426A42DC8B7}"/>
+    <hyperlink ref="F20" r:id="rId22" xr:uid="{E3458C57-673F-4CB9-8F10-A99A4FE90CA8}"/>
+    <hyperlink ref="F6" r:id="rId23" xr:uid="{0573C17F-D69B-424E-8488-23BA74D33C8B}"/>
+    <hyperlink ref="F11" r:id="rId24" xr:uid="{4D0AE52B-41FB-4D05-8701-741335AE2CE0}"/>
+    <hyperlink ref="F30" r:id="rId25" xr:uid="{86068225-93F0-4B5A-BC4C-381A0D7D6680}"/>
+    <hyperlink ref="F31" r:id="rId26" xr:uid="{9B2FB9CE-4C44-4EE2-B5CB-FE703EFF1135}"/>
+    <hyperlink ref="F32" r:id="rId27" xr:uid="{8F6C8324-ED29-48DE-AE3D-8BDBF9E62963}"/>
+    <hyperlink ref="F33" r:id="rId28" xr:uid="{43011799-FE31-4CFC-B29F-CE5CD44B1568}"/>
+    <hyperlink ref="F24" r:id="rId29" xr:uid="{81EB3D8B-1797-4B33-9B13-10350F56C940}"/>
+    <hyperlink ref="F25" r:id="rId30" xr:uid="{A72DB0DC-11A8-4BA0-9440-4001558EC991}"/>
+    <hyperlink ref="F26" r:id="rId31" xr:uid="{A36A8DC8-F555-43C6-BD5C-71355E27128C}"/>
+    <hyperlink ref="F4" r:id="rId32" xr:uid="{61F36960-8749-4413-B44B-B18C3D1C1259}"/>
+    <hyperlink ref="F8" r:id="rId33" xr:uid="{34C08891-5177-41BE-9B56-875E550EF5D2}"/>
+    <hyperlink ref="F13" r:id="rId34" xr:uid="{109344F1-083B-4340-9DDD-776CCE34C0D0}"/>
+    <hyperlink ref="F14" r:id="rId35" xr:uid="{34DB9349-8FB3-487F-BF43-8BD752B201B0}"/>
+    <hyperlink ref="F21" r:id="rId36" xr:uid="{15167636-5261-460F-A387-38041120A653}"/>
+    <hyperlink ref="F42" r:id="rId37" xr:uid="{1EC25666-66C9-4D4F-90AD-0039691DBD8D}"/>
+    <hyperlink ref="F43" r:id="rId38" xr:uid="{6ACCA3AE-5E4B-4D37-A2D4-5460BC29F0D0}"/>
+    <hyperlink ref="F27" r:id="rId39" xr:uid="{3AA03225-89D6-4BC7-A423-32B694A0D34A}"/>
+    <hyperlink ref="F28" r:id="rId40" xr:uid="{8A788927-523F-423C-8A9C-7B7D4E5466A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId41"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>